<commit_message>
doc: Save results data size vs performance study
</commit_message>
<xml_diff>
--- a/scratch/2017-01-23-lhof-performance_vs_data_size_graph.xlsx
+++ b/scratch/2017-01-23-lhof-performance_vs_data_size_graph.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5020" yWindow="4780" windowWidth="27400" windowHeight="16820" tabRatio="500"/>
+    <workbookView xWindow="1120" yWindow="3420" windowWidth="27400" windowHeight="16820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -161,7 +161,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0608813817627635"/>
+          <c:y val="0.0918763326226013"/>
+          <c:w val="0.907378447388474"/>
+          <c:h val="0.804555680539932"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -205,10 +215,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.99</c:v>
                 </c:pt>
@@ -238,16 +248,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:f>Sheet1!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.7444</c:v>
                 </c:pt>
@@ -277,6 +290,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.8777</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>0.831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -323,10 +339,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.99</c:v>
                 </c:pt>
@@ -356,16 +372,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$11</c:f>
+              <c:f>Sheet1!$E$2:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.6893191</c:v>
                 </c:pt>
@@ -395,6 +414,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.643744</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.6916667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -441,10 +463,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.99</c:v>
                 </c:pt>
@@ -474,16 +496,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$11</c:f>
+              <c:f>Sheet1!$F$2:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.7339</c:v>
                 </c:pt>
@@ -513,6 +538,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.6908</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.6183</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -527,11 +555,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="807864304"/>
-        <c:axId val="753668000"/>
+        <c:axId val="811124560"/>
+        <c:axId val="811126608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="807864304"/>
+        <c:axId val="811124560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -587,12 +615,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="753668000"/>
+        <c:crossAx val="811126608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="753668000"/>
+        <c:axId val="811126608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -614,6 +642,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -650,7 +679,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="807864304"/>
+        <c:crossAx val="811124560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1585,10 +1614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R35" sqref="R35"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1912,6 +1941,38 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1133</v>
+      </c>
+      <c r="C12" s="1">
+        <v>47</v>
+      </c>
+      <c r="D12">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="E12">
+        <v>0.69166669999999997</v>
+      </c>
+      <c r="F12">
+        <v>0.61829999999999996</v>
+      </c>
+      <c r="G12">
+        <v>400</v>
+      </c>
+      <c r="H12">
+        <v>6</v>
+      </c>
+      <c r="I12">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C13" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>